<commit_message>
Added functionality to be able to check todays date against pay period date
</commit_message>
<xml_diff>
--- a/AVbook.xlsx
+++ b/AVbook.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git_workspaces\py_program\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D336FE8B-38F2-4C4D-AF4A-5FC838165D60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B96C6C3C-52A1-4801-9094-E64A84869040}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{FF0A48C2-EF76-4B1E-85B2-E0F9510F4968}"/>
   </bookViews>
@@ -65,8 +65,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -381,12 +382,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22C286A4-0D5F-4849-A6FE-05D986FD1A64}">
-  <dimension ref="A1"/>
+  <dimension ref="E1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="5" max="5" width="9.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E1" s="1">
+        <v>44711</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>